<commit_message>
Figure and manuscript updates
</commit_message>
<xml_diff>
--- a/sch_results.xlsx
+++ b/sch_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/be82ef303f3cad60/Systems Science/Lab/Necessary Heterogenity in Network Models of Residential Segregation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_496D5DA7037A7CEEE065DCF650245E3FB48F8B4D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A410457-97AF-439E-ABB2-2A1CE33540DB}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_496D048F0060545FE659BC3557245E3FB48F8B5C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D59BF984-E473-4324-A8D1-923FABF5418B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="H6" sqref="B2:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,22 +446,22 @@
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <v>0.6782061358335838</v>
+        <v>0.88036686785260754</v>
       </c>
       <c r="D2" s="2">
-        <v>2.3398509274099848E-2</v>
+        <v>1.620901189538734E-2</v>
       </c>
       <c r="E2" s="2">
-        <v>1.1499999999999999</v>
+        <v>2.94</v>
       </c>
       <c r="F2" s="2">
-        <v>0.38405728739343042</v>
+        <v>1.4547852075134671</v>
       </c>
       <c r="G2" s="2">
-        <v>3.6138608689853129E-3</v>
+        <v>3.7868582671209748E-3</v>
       </c>
       <c r="H2" s="2">
-        <v>4.8766158893920069E-5</v>
+        <v>2.399945072882051E-5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -472,22 +472,22 @@
         <v>32</v>
       </c>
       <c r="C3" s="2">
-        <v>0.78308173553284677</v>
+        <v>0.94272746487918568</v>
       </c>
       <c r="D3" s="2">
-        <v>7.7044055671976225E-2</v>
+        <v>1.0346402372290901E-2</v>
       </c>
       <c r="E3" s="2">
-        <v>1.76</v>
+        <v>2.67</v>
       </c>
       <c r="F3" s="2">
-        <v>1.32</v>
+        <v>1.2414104881142261</v>
       </c>
       <c r="G3" s="2">
-        <v>1.104808557383377E-2</v>
+        <v>5.8193382476187331E-3</v>
       </c>
       <c r="H3" s="2">
-        <v>1.3196941445204121E-3</v>
+        <v>5.7047463655118022E-4</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -498,22 +498,22 @@
         <v>64</v>
       </c>
       <c r="C4" s="2">
-        <v>0.65235554086183445</v>
+        <v>0.95027287165552976</v>
       </c>
       <c r="D4" s="2">
-        <v>0.14468135541062541</v>
+        <v>1.089658272263714E-2</v>
       </c>
       <c r="E4" s="2">
-        <v>2.44</v>
+        <v>2.39</v>
       </c>
       <c r="F4" s="2">
-        <v>1.402283851436648</v>
+        <v>1.018773772728764</v>
       </c>
       <c r="G4" s="2">
-        <v>1.399358610301661E-2</v>
+        <v>8.6680309727733881E-3</v>
       </c>
       <c r="H4" s="2">
-        <v>9.2629778363405941E-4</v>
+        <v>7.8378403568300737E-4</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -524,22 +524,22 @@
         <v>96</v>
       </c>
       <c r="C5" s="2">
-        <v>0.57269553694299491</v>
+        <v>0.94877935351053</v>
       </c>
       <c r="D5" s="2">
-        <v>0.15885434050600511</v>
+        <v>1.2615406843775609E-2</v>
       </c>
       <c r="E5" s="2">
-        <v>2.2599999999999998</v>
+        <v>2.16</v>
       </c>
       <c r="F5" s="2">
-        <v>1.3610290224679269</v>
+        <v>1.1110355529864919</v>
       </c>
       <c r="G5" s="2">
-        <v>1.5707651245558729E-2</v>
+        <v>1.1403179855917539E-2</v>
       </c>
       <c r="H5" s="2">
-        <v>9.3428731647683401E-4</v>
+        <v>8.7581676481739146E-4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -550,22 +550,22 @@
         <v>128</v>
       </c>
       <c r="C6" s="2">
-        <v>0.51837893609827679</v>
+        <v>0.94383765778470829</v>
       </c>
       <c r="D6" s="2">
-        <v>0.15784778042227379</v>
+        <v>1.437875586706742E-2</v>
       </c>
       <c r="E6" s="2">
-        <v>1.84</v>
+        <v>1.86</v>
       </c>
       <c r="F6" s="2">
-        <v>0.99719606898543289</v>
+        <v>0.92757749002441814</v>
       </c>
       <c r="G6" s="2">
-        <v>1.7365335666926121E-2</v>
+        <v>1.3974061868830569E-2</v>
       </c>
       <c r="H6" s="2">
-        <v>1.0028096044098871E-3</v>
+        <v>9.881182744139903E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>